<commit_message>
DEV: Updated output Files
</commit_message>
<xml_diff>
--- a/DataAnalysis/Data/output/makro_analysis.xlsx
+++ b/DataAnalysis/Data/output/makro_analysis.xlsx
@@ -882,7 +882,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7">
@@ -922,7 +922,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="n">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="12">
@@ -930,7 +930,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>1092</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="13">
@@ -938,7 +938,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="n">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="14">
@@ -946,7 +946,7 @@
         <v>24</v>
       </c>
       <c r="B14" t="n">
-        <v>855</v>
+        <v>852</v>
       </c>
     </row>
     <row r="15">
@@ -954,7 +954,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="n">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16">
@@ -962,7 +962,7 @@
         <v>28</v>
       </c>
       <c r="B16" t="n">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17">
@@ -970,7 +970,7 @@
         <v>30</v>
       </c>
       <c r="B17" t="n">
-        <v>356</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18">
@@ -978,7 +978,7 @@
         <v>32</v>
       </c>
       <c r="B18" t="n">
-        <v>148</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19">
@@ -986,7 +986,7 @@
         <v>34</v>
       </c>
       <c r="B19" t="n">
-        <v>305</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20">
@@ -994,7 +994,7 @@
         <v>36</v>
       </c>
       <c r="B20" t="n">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21">
@@ -1002,7 +1002,7 @@
         <v>38</v>
       </c>
       <c r="B21" t="n">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22">
@@ -1010,7 +1010,7 @@
         <v>40</v>
       </c>
       <c r="B22" t="n">
-        <v>286</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23">
@@ -1018,7 +1018,7 @@
         <v>42</v>
       </c>
       <c r="B23" t="n">
-        <v>116</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24">
@@ -1026,7 +1026,7 @@
         <v>44</v>
       </c>
       <c r="B24" t="n">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25">
@@ -1034,7 +1034,7 @@
         <v>46</v>
       </c>
       <c r="B25" t="n">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26">
@@ -1042,7 +1042,7 @@
         <v>48</v>
       </c>
       <c r="B26" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27">
@@ -1050,7 +1050,7 @@
         <v>50</v>
       </c>
       <c r="B27" t="n">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28">
@@ -1058,7 +1058,7 @@
         <v>52</v>
       </c>
       <c r="B28" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29">
@@ -1066,7 +1066,7 @@
         <v>54</v>
       </c>
       <c r="B29" t="n">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30">
@@ -1082,7 +1082,7 @@
         <v>58</v>
       </c>
       <c r="B31" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32">
@@ -1090,7 +1090,7 @@
         <v>60</v>
       </c>
       <c r="B32" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33">
@@ -1193,7 +1193,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3">
@@ -1201,7 +1201,7 @@
         <v>50</v>
       </c>
       <c r="B3" t="n">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4">
@@ -1217,7 +1217,7 @@
         <v>150</v>
       </c>
       <c r="B5" t="n">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
@@ -1225,7 +1225,7 @@
         <v>200</v>
       </c>
       <c r="B6" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7">
@@ -1233,7 +1233,7 @@
         <v>250</v>
       </c>
       <c r="B7" t="n">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8">
@@ -1241,7 +1241,7 @@
         <v>300</v>
       </c>
       <c r="B8" t="n">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9">
@@ -1249,7 +1249,7 @@
         <v>350</v>
       </c>
       <c r="B9" t="n">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10">
@@ -1257,7 +1257,7 @@
         <v>400</v>
       </c>
       <c r="B10" t="n">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="11">
@@ -1265,7 +1265,7 @@
         <v>450</v>
       </c>
       <c r="B11" t="n">
-        <v>635</v>
+        <v>624</v>
       </c>
     </row>
     <row r="12">
@@ -1273,7 +1273,7 @@
         <v>500</v>
       </c>
       <c r="B12" t="n">
-        <v>795</v>
+        <v>790</v>
       </c>
     </row>
     <row r="13">
@@ -1281,7 +1281,7 @@
         <v>550</v>
       </c>
       <c r="B13" t="n">
-        <v>827</v>
+        <v>819</v>
       </c>
     </row>
     <row r="14">
@@ -1289,7 +1289,7 @@
         <v>600</v>
       </c>
       <c r="B14" t="n">
-        <v>856</v>
+        <v>841</v>
       </c>
     </row>
     <row r="15">
@@ -1297,7 +1297,7 @@
         <v>650</v>
       </c>
       <c r="B15" t="n">
-        <v>862</v>
+        <v>840</v>
       </c>
     </row>
     <row r="16">
@@ -1305,7 +1305,7 @@
         <v>700</v>
       </c>
       <c r="B16" t="n">
-        <v>593</v>
+        <v>572</v>
       </c>
     </row>
     <row r="17">
@@ -1313,7 +1313,7 @@
         <v>750</v>
       </c>
       <c r="B17" t="n">
-        <v>503</v>
+        <v>483</v>
       </c>
     </row>
     <row r="18">
@@ -1321,7 +1321,7 @@
         <v>800</v>
       </c>
       <c r="B18" t="n">
-        <v>410</v>
+        <v>388</v>
       </c>
     </row>
     <row r="19">
@@ -1329,7 +1329,7 @@
         <v>850</v>
       </c>
       <c r="B19" t="n">
-        <v>315</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20">
@@ -1337,7 +1337,7 @@
         <v>900</v>
       </c>
       <c r="B20" t="n">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21">
@@ -1345,7 +1345,7 @@
         <v>950</v>
       </c>
       <c r="B21" t="n">
-        <v>201</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22">
@@ -1353,7 +1353,7 @@
         <v>1000</v>
       </c>
       <c r="B22" t="n">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23">
@@ -1361,7 +1361,7 @@
         <v>1050</v>
       </c>
       <c r="B23" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24">
@@ -1369,7 +1369,7 @@
         <v>1100</v>
       </c>
       <c r="B24" t="n">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25">
@@ -1377,7 +1377,7 @@
         <v>1150</v>
       </c>
       <c r="B25" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26">
@@ -1385,7 +1385,7 @@
         <v>1200</v>
       </c>
       <c r="B26" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27">
@@ -1393,7 +1393,7 @@
         <v>1250</v>
       </c>
       <c r="B27" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28">
@@ -1409,7 +1409,7 @@
         <v>1350</v>
       </c>
       <c r="B29" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30">
@@ -1417,7 +1417,7 @@
         <v>1400</v>
       </c>
       <c r="B30" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31">
@@ -1433,7 +1433,7 @@
         <v>1500</v>
       </c>
       <c r="B32" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33">
@@ -1576,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3">
@@ -1584,7 +1584,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4">
@@ -1592,7 +1592,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
@@ -1600,7 +1600,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6">
@@ -1608,7 +1608,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7">
@@ -1616,7 +1616,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8">
@@ -1624,7 +1624,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="n">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9">
@@ -1632,7 +1632,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>227</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10">
@@ -1640,7 +1640,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="n">
-        <v>329</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11">
@@ -1648,7 +1648,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="n">
-        <v>360</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12">
@@ -1656,7 +1656,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>532</v>
+        <v>504</v>
       </c>
     </row>
     <row r="13">
@@ -1664,7 +1664,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="n">
-        <v>548</v>
+        <v>524</v>
       </c>
     </row>
     <row r="14">
@@ -1672,7 +1672,7 @@
         <v>24</v>
       </c>
       <c r="B14" t="n">
-        <v>601</v>
+        <v>572</v>
       </c>
     </row>
     <row r="15">
@@ -1680,7 +1680,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="n">
-        <v>606</v>
+        <v>589</v>
       </c>
     </row>
     <row r="16">
@@ -1688,7 +1688,7 @@
         <v>28</v>
       </c>
       <c r="B16" t="n">
-        <v>438</v>
+        <v>425</v>
       </c>
     </row>
     <row r="17">
@@ -1696,7 +1696,7 @@
         <v>30</v>
       </c>
       <c r="B17" t="n">
-        <v>565</v>
+        <v>558</v>
       </c>
     </row>
     <row r="18">
@@ -1704,7 +1704,7 @@
         <v>32</v>
       </c>
       <c r="B18" t="n">
-        <v>520</v>
+        <v>514</v>
       </c>
     </row>
     <row r="19">
@@ -1712,7 +1712,7 @@
         <v>34</v>
       </c>
       <c r="B19" t="n">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="20">
@@ -1728,7 +1728,7 @@
         <v>38</v>
       </c>
       <c r="B21" t="n">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="22">
@@ -1736,7 +1736,7 @@
         <v>40</v>
       </c>
       <c r="B22" t="n">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23">
@@ -1744,7 +1744,7 @@
         <v>42</v>
       </c>
       <c r="B23" t="n">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24">
@@ -1752,7 +1752,7 @@
         <v>44</v>
       </c>
       <c r="B24" t="n">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25">
@@ -1776,7 +1776,7 @@
         <v>50</v>
       </c>
       <c r="B27" t="n">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28">
@@ -1792,7 +1792,7 @@
         <v>54</v>
       </c>
       <c r="B29" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30">
@@ -1880,7 +1880,7 @@
         <v>76</v>
       </c>
       <c r="B40" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41">

</xml_diff>